<commit_message>
merging the scraper with the crime analyzer script (along with the output files)
</commit_message>
<xml_diff>
--- a/regular_meetings_v2.0.xlsx
+++ b/regular_meetings_v2.0.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regular Meetings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="301">
   <si>
     <t>Meeting #</t>
   </si>
@@ -34,6 +34,12 @@
     <t>Meeting Page</t>
   </si>
   <si>
+    <t>Chief Verbal Report Present</t>
+  </si>
+  <si>
+    <t>Verbal Report File URL</t>
+  </si>
+  <si>
     <t>November 28, 2022</t>
   </si>
   <si>
@@ -88,9 +94,6 @@
     <t>January 25, 2021</t>
   </si>
   <si>
-    <t>December 21, 2020</t>
-  </si>
-  <si>
     <t>November 23, 2020</t>
   </si>
   <si>
@@ -109,9 +112,6 @@
     <t>April 27, 2020</t>
   </si>
   <si>
-    <t>March 23, 2020</t>
-  </si>
-  <si>
     <t>February 24, 2020</t>
   </si>
   <si>
@@ -298,9 +298,6 @@
     <t>January 27, 2014</t>
   </si>
   <si>
-    <t>December 16, 2013</t>
-  </si>
-  <si>
     <t>November 25, 2013</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>March 25, 2013</t>
   </si>
   <si>
-    <t>February 25, 2013</t>
-  </si>
-  <si>
     <t>January 28, 2013</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
     <t>Via Zoom</t>
   </si>
   <si>
-    <t>CANCELLED</t>
-  </si>
-  <si>
     <t>Council Chambers</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>2:00 p.m.</t>
   </si>
   <si>
-    <t>16 h</t>
-  </si>
-  <si>
     <t>9:30 a.m</t>
   </si>
   <si>
@@ -502,9 +490,6 @@
     <t>https://pub-ottawa.escribemeetings.com/Meeting.aspx?Id=462ae882-415d-46a0-5107-00a87e534a6c&amp;Agenda=Agenda&amp;lang=English</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>https://pub-ottawa.escribemeetings.com/Meeting.aspx?Id=713a95ba-6398-6f2f-645a-a80e1db79baa&amp;Agenda=Agenda&amp;lang=English</t>
   </si>
   <si>
@@ -797,6 +782,141 @@
   </si>
   <si>
     <t>http://ottawa.ca/cgi-bin/docs.pl?Elist=16206&amp;lang=en</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103234', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103235', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103236', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103237', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103241', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103238', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103239', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103242', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=103240']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100090', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100091', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100106', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100107', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100092', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100093', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100094', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100095', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100096', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100097', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100098', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100099', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100100', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100101', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100102', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=100104']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97934', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97906', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97907', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97908', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97909', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97910', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97911', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97912', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97913', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97914', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97915', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97916', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97917', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97918', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97919', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97920', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97921', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97922', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97923', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=97925']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=91639', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=91637']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74722', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74697', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74698', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74699', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74703', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74704', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74705', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74706', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74712', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74713', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74714', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74715', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74716', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74717', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74707', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74708', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74709', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74710', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74711', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=74693']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78385', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78386', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78387', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78388', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78389', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78390', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78391', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78392', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78393', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78394', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78395', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78396', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78397', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78398', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78399', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78400', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78401', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78402', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78403', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78404', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78405', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78406', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=78408']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6288', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6289', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6290', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6291', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6292', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6293', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6294', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6295', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6296', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6297', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6298', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6299', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6300', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6301', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?DocumentId=6302']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88163', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88164', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88165', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88166', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88167', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88168', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88169', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88170', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88171', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88172', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=88175']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86986', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86987', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86988', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86989', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86990', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87009', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87010', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87011', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87012', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87013', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87014', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87015', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87016', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87017', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87018', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87019', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87020', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=87025']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86943', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86944', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86945', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86946', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86947', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86948', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86949', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86950', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86952', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86940', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86953', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86954', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86955', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86956', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86957', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86958', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86959', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86960', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86961', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86962', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86963', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86964', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86965']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86908', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86909', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86910', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86911', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86915', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86916', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86917', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86918', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86919', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86920', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86921', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86922', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86923', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86924', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86925', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86926', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86927', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86928', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86932']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86876', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86882', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86883', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86884', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86885', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86886', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86887', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86888', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86889', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86890', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86891', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86892', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86894']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86828', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86832', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86833', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86834', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86835', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=86837']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49940', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49953', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49954', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49955', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49956', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49957', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49958', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49959', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49960', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49961', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49962', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49963', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49964', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49965', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49966', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49967', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=49969']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31898', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31900', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31901', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31902', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31905', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31906', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31907', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31908', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31909', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=31913']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60362', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60367', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60368', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60369', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60370', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60371', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60373', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60374', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60375', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60376', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60377', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60378', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60379', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60380', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60381', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60382', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=60384']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21282', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21283', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21284', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21289', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21290', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21291', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21292', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21293', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21294', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21295', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21296', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21297', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21298', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21299', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21300', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21301', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21302', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21305']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57099', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57103', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57104', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57105', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57106', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57107', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57108', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57109', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57110', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57111', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57112', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57113', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57114', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57115', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57116', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57117', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57118', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57119', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57120', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57121', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57122', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57123', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57124', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57130']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50469', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50470', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50471', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50472', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50473', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50474', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50475', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50476', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50477', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50480', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50481', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50482', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50483', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50484', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50485', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50486', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50487', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50488', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50489', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50490', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50491', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50492', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50493', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50494', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50495', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50496', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=50498']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=55885']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41069', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41076', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41077', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41078', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41080', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41088', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41089', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41090', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41091', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41092', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41093', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41095']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34600', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34601', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34605', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34606', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34607', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34608', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34609', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34610', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34612', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34613', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34614', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34615', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34616', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34617', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34640', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34637', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34638', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34639', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34600', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34601', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34602', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34603', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34604', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34605', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34606', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34607', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34608', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34609', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34610', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34611', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34612', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34613', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34614', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34615', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34616', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34617', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34618', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34619', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34620', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34621', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34622', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=34629']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61852', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61853', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61854']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28326', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28330', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28335', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28336', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28337', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28338', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28339', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28340', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28341', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28342', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28343', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28344', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28345', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28346', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28347', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=28351']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61676']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54528', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54529', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54530', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54531', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54532', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54557', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54558', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54533', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54534', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54535', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54536', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54541', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54542', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54543', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54544', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54550', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54551', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54537', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54552', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54553', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54554', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54555', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=54556']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41445', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41448', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41449', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41450', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41451', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41452', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41453', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41454', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41455', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41456', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=41457']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21349', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21350', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21351', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21356', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21357', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21358', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21359', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21360', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=21363']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52613', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52614', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52615', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52616', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52617', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52618', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52619', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52620', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52621', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52622', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52623', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52624', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52625', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52626', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52627', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52628', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52629', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52630', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52631', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52637', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52637', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52637', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52637', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52632', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52633', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52634', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52635', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52636', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=52637']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27595', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27596', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27597', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27598']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35681', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35682', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65545', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65546', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35681', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35682', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35683', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35688', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35689', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35690', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35691', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35692', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35693', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35686', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35687', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35684', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35694', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35679', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35680', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35685', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35695', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35686', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35687', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35684', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35694', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35679', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35680', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35685', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35695', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35686', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35687', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35684', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35694', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35679', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35680', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35685', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35695', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35686', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35687', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35684', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35694', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35679', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35680', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35685', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35695', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35686', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35687', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35684', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35694', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35679', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35680', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35685', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35695', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=35667']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57839', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57840', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57841', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57842', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27202', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27203', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27204', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27205', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27206', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27207', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27208', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27209', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27210', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27211', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27212', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27213', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27214', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27215', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27216', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27217', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27218', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27219', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27220', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27221', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27222', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27223', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27224', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57839', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57840', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57841', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57842', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27202', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27203', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27204', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27205', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27206', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27207', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27208', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27209', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27210', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27211', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27212', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27213', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27214', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27215', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27216', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27217', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27218', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27219', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27220', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27221', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27222', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27223', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27224', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57839', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57840', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57841', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57842', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27202', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27203', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27204', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27205', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27206', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27207', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27208', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27209', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27210', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27211', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27212', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27213', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27214', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27215', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27216', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27217', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27218', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27219', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27220', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27221', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27222', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27223', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27224', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57839', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57840', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57841', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57842', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27202', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27203', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27204', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27205', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27206', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27207', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27208', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27209', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27210', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27211', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27212', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27213', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27214', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27215', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27216', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27217', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27218', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27219', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27220', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27221', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27222', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27223', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27224', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57839', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57840', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57841', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=57842', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27202', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27203', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27204', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27205', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27206', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27207', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27208', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27209', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27210', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27211', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27212', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27213', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27214', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27215', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27216', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27217', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27218', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27219', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27220', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27221', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27222', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27223', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=27224']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51052', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51037', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51038', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51042', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51043', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51044', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51045', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51046', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51047', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51057', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51048', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51050']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61084', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61085', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61086', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61080', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61084', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61085', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61086', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61080', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61084', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61085', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61086', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61080', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61084', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61085', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61086', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61080', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61083', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61084', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61085', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61086', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61082', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61081', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61087', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61079', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61080']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33417', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33425', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33419', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33420', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33421', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33415', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33410', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33411', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33426', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33427', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33412', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33413', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33418', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33414', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33422', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33423', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33424', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33416', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33414', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33422', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33423', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33424', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=33416']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39539', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39548', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39549', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39538', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39547', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39540', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=39541']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65476', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65477', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62065', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62066', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62068', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65496', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62067', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65493', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65478', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65479', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65497', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65498', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65476', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65477', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62065', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62066', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62068', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65496', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62067', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65493', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65478', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65479', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65497', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65498', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65476', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65477', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62065', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62066', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62068', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65496', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=62067', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65493', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65478', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65479', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65497', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65498', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65485', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65486', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65487', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65480', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65481', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65482', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65483', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65484', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65485', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65486', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65487', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65480', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65481', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65482', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65483', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65484', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65485', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65486', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65487', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65480', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65481', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65482', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65483', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65484', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65485', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65486', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65487', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65480', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65481', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65482', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65483', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65484', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65488', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65489', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65490', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65491', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65492', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65494', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65495', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65943', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65488', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65489', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65490', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65491', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65492', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65494', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65495', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65943', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65488', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65489', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65490', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65491', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65492', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65494', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65495', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=65943']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61143', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61145', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61144', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61164', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61165', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61163', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61155', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61160', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61161', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61156', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61157', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61158', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61159', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61162', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61152', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61153', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61154', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61148', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61151', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61150', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61146', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61149', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61147']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63581', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63582', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63583', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63586', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63587', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63580', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63584', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63585', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63599', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63588']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=51669']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61874', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61875', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61876', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61877', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61878', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61873', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=61867']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32768', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32760', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32762', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32767', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32761', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32763', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32764', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32765', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32766', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32768', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32760', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32762', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32767', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32761', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32763', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32764', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32765', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32766', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32768', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32760', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32762', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32767', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32761', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32763', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32764', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32765', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32766', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32768', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32760', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32762', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32767', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32761', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32763', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32764', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32765', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=32766']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67658', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67659', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67660', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67663', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63996', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63997', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64002', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64003', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64004', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64005', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64006', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64007', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64008', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63998', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=63999', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67661', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67662', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64000', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=64001', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67673', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67674', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67675', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67676', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67677', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67678', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67666', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67664', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67665', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=68885', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67666', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67664', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67665', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=68885', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67667', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67668', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67669', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67670', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67671', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67672', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67666', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67664', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=67665', 'https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=68885']</t>
+  </si>
+  <si>
+    <t>['https://pub-ottawa.escribemeetings.com/filestream.ashx?documentid=44265']</t>
   </si>
 </sst>
 </file>
@@ -1167,13 +1287,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1192,8 +1312,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1201,22 +1327,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1224,22 +1356,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>141</v>
+      </c>
+      <c r="H3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1247,22 +1385,28 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>256</v>
+      </c>
+      <c r="I4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1270,22 +1414,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1293,22 +1443,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>144</v>
+      </c>
+      <c r="H6" t="s">
+        <v>256</v>
+      </c>
+      <c r="I6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1316,22 +1472,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>145</v>
+      </c>
+      <c r="H7" t="s">
+        <v>256</v>
+      </c>
+      <c r="I7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1339,22 +1501,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>146</v>
+      </c>
+      <c r="H8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1362,22 +1530,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>147</v>
+      </c>
+      <c r="H9" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1385,22 +1559,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>148</v>
+      </c>
+      <c r="H10" t="s">
+        <v>256</v>
+      </c>
+      <c r="I10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1408,22 +1588,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>149</v>
+      </c>
+      <c r="H11" t="s">
+        <v>256</v>
+      </c>
+      <c r="I11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1431,22 +1617,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>150</v>
+      </c>
+      <c r="H12" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1454,22 +1646,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>151</v>
+      </c>
+      <c r="H13" t="s">
+        <v>256</v>
+      </c>
+      <c r="I13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1477,22 +1675,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>152</v>
+      </c>
+      <c r="H14" t="s">
+        <v>256</v>
+      </c>
+      <c r="I14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1500,22 +1704,28 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>153</v>
+      </c>
+      <c r="H15" t="s">
+        <v>256</v>
+      </c>
+      <c r="I15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1523,22 +1733,28 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>154</v>
+      </c>
+      <c r="H16" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1546,22 +1762,28 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>155</v>
+      </c>
+      <c r="H17" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1569,22 +1791,28 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>156</v>
+      </c>
+      <c r="H18" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1592,1422 +1820,1584 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>157</v>
+      </c>
+      <c r="H19" t="s">
+        <v>256</v>
+      </c>
+      <c r="I19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>139</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" t="s">
+        <v>256</v>
+      </c>
+      <c r="I20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>159</v>
+      </c>
+      <c r="H21" t="s">
+        <v>256</v>
+      </c>
+      <c r="I21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>160</v>
+      </c>
+      <c r="H22" t="s">
+        <v>256</v>
+      </c>
+      <c r="I22" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>161</v>
+      </c>
+      <c r="H23" t="s">
+        <v>256</v>
+      </c>
+      <c r="I23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>162</v>
+      </c>
+      <c r="H24" t="s">
+        <v>256</v>
+      </c>
+      <c r="I24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>163</v>
+      </c>
+      <c r="H25" t="s">
+        <v>256</v>
+      </c>
+      <c r="I25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>164</v>
+      </c>
+      <c r="H26" t="s">
+        <v>256</v>
+      </c>
+      <c r="I26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E27" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>139</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H27" t="s">
+        <v>256</v>
+      </c>
+      <c r="I27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>166</v>
+      </c>
+      <c r="H28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>167</v>
+      </c>
+      <c r="H29" t="s">
+        <v>256</v>
+      </c>
+      <c r="I29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>168</v>
+      </c>
+      <c r="H30" t="s">
+        <v>256</v>
+      </c>
+      <c r="I30" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>170</v>
+      </c>
+      <c r="H32" t="s">
+        <v>256</v>
+      </c>
+      <c r="I32" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>171</v>
+      </c>
+      <c r="H33" t="s">
+        <v>256</v>
+      </c>
+      <c r="I33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>172</v>
+      </c>
+      <c r="H34" t="s">
+        <v>256</v>
+      </c>
+      <c r="I34" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>174</v>
+      </c>
+      <c r="H36" t="s">
+        <v>256</v>
+      </c>
+      <c r="I36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
         <v>125</v>
       </c>
       <c r="E37" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>175</v>
+      </c>
+      <c r="H37" t="s">
+        <v>256</v>
+      </c>
+      <c r="I37" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F38" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>177</v>
+      </c>
+      <c r="H39" t="s">
+        <v>256</v>
+      </c>
+      <c r="I39" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>178</v>
+      </c>
+      <c r="H40" t="s">
+        <v>256</v>
+      </c>
+      <c r="I40" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F41" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>179</v>
+      </c>
+      <c r="H41" t="s">
+        <v>256</v>
+      </c>
+      <c r="I41" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>180</v>
+      </c>
+      <c r="H42" t="s">
+        <v>256</v>
+      </c>
+      <c r="I42" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F43" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F44" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>183</v>
+      </c>
+      <c r="H45" t="s">
+        <v>256</v>
+      </c>
+      <c r="I45" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F46" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F47" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>185</v>
+      </c>
+      <c r="H47" t="s">
+        <v>256</v>
+      </c>
+      <c r="I47" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E48" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F48" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E49" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>187</v>
+      </c>
+      <c r="H49" t="s">
+        <v>256</v>
+      </c>
+      <c r="I49" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E50" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>188</v>
+      </c>
+      <c r="H50" t="s">
+        <v>256</v>
+      </c>
+      <c r="I50" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>190</v>
+      </c>
+      <c r="H52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I52" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F55" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
         <v>134</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E59" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F59" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E60" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F60" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E61" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F61" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D62" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E62" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F62" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E63" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E64" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E65" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F65" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E66" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E67" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F67" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E68" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>206</v>
+      </c>
+      <c r="H68" t="s">
+        <v>256</v>
+      </c>
+      <c r="I68" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E69" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F69" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F70" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E72" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F72" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D73" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D76" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F76" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D77" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E77" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F77" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F78" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D79" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E79" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F79" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D80" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E80" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F80" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3015,22 +3405,22 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D81" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F81" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3038,22 +3428,22 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D82" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F82" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3061,22 +3451,22 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C83" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D83" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E83" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F83" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3084,22 +3474,22 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C84" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F84" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3107,22 +3497,22 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C85" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E85" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F85" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3130,22 +3520,22 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C86" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E86" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F86" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3153,22 +3543,22 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C87" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D87" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E87" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F87" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3176,22 +3566,22 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E88" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F88" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3199,22 +3589,22 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D89" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E89" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F89" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3222,22 +3612,22 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D90" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E90" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F90" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3245,19 +3635,22 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D91" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E91" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F91" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -3265,22 +3658,22 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D92" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E92" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F92" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3288,22 +3681,22 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E93" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F93" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3311,22 +3704,22 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E94" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F94" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3334,22 +3727,22 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E95" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F95" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3357,22 +3750,22 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D96" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E96" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F96" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3380,22 +3773,22 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D97" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E97" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F97" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3403,22 +3796,22 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E98" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F98" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -3426,22 +3819,22 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C99" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D99" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E99" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F99" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3449,19 +3842,22 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D100" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E100" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F100" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3469,22 +3865,22 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D101" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F101" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3492,22 +3888,22 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D102" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E102" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F102" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3515,22 +3911,22 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D103" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E103" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F103" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3538,22 +3934,22 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C104" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D104" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E104" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F104" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3561,22 +3957,22 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D105" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E105" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F105" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3584,22 +3980,22 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E106" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F106" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3607,22 +4003,22 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C107" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D107" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E107" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F107" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3630,22 +4026,22 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C108" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D108" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E108" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F108" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3653,22 +4049,22 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C109" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D109" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E109" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F109" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3676,22 +4072,22 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C110" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D110" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E110" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F110" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3699,22 +4095,22 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D111" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E111" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F111" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3722,22 +4118,22 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C112" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D112" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E112" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F112" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3745,22 +4141,22 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D113" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E113" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F113" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3768,22 +4164,22 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C114" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D114" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E114" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F114" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3791,22 +4187,22 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D115" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E115" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F115" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3814,22 +4210,22 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C116" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D116" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E116" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F116" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3837,114 +4233,22 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C117" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D117" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E117" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F117" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="1">
-        <v>116</v>
-      </c>
-      <c r="B118">
-        <v>117</v>
-      </c>
-      <c r="C118" t="s">
-        <v>121</v>
-      </c>
-      <c r="D118" t="s">
-        <v>125</v>
-      </c>
-      <c r="E118" t="s">
-        <v>142</v>
-      </c>
-      <c r="F118" t="s">
-        <v>143</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119">
-        <v>118</v>
-      </c>
-      <c r="C119" t="s">
-        <v>122</v>
-      </c>
-      <c r="D119" t="s">
-        <v>125</v>
-      </c>
-      <c r="E119" t="s">
-        <v>142</v>
-      </c>
-      <c r="F119" t="s">
-        <v>143</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="1">
-        <v>118</v>
-      </c>
-      <c r="B120">
-        <v>119</v>
-      </c>
-      <c r="C120" t="s">
-        <v>123</v>
-      </c>
-      <c r="D120" t="s">
-        <v>125</v>
-      </c>
-      <c r="E120" t="s">
-        <v>142</v>
-      </c>
-      <c r="F120" t="s">
-        <v>143</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="A121" s="1">
-        <v>119</v>
-      </c>
-      <c r="B121">
-        <v>120</v>
-      </c>
-      <c r="C121" t="s">
-        <v>124</v>
-      </c>
-      <c r="D121" t="s">
-        <v>125</v>
-      </c>
-      <c r="E121" t="s">
-        <v>142</v>
-      </c>
-      <c r="F121" t="s">
-        <v>143</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3967,104 +4271,104 @@
     <hyperlink ref="G17" r:id="rId16"/>
     <hyperlink ref="G18" r:id="rId17"/>
     <hyperlink ref="G19" r:id="rId18"/>
-    <hyperlink ref="G21" r:id="rId19"/>
-    <hyperlink ref="G22" r:id="rId20"/>
-    <hyperlink ref="G23" r:id="rId21"/>
-    <hyperlink ref="G24" r:id="rId22"/>
-    <hyperlink ref="G25" r:id="rId23"/>
-    <hyperlink ref="G26" r:id="rId24"/>
-    <hyperlink ref="G28" r:id="rId25"/>
-    <hyperlink ref="G29" r:id="rId26"/>
-    <hyperlink ref="G30" r:id="rId27"/>
-    <hyperlink ref="G31" r:id="rId28"/>
-    <hyperlink ref="G32" r:id="rId29"/>
-    <hyperlink ref="G33" r:id="rId30"/>
-    <hyperlink ref="G34" r:id="rId31"/>
-    <hyperlink ref="G35" r:id="rId32"/>
-    <hyperlink ref="G36" r:id="rId33"/>
-    <hyperlink ref="G37" r:id="rId34"/>
-    <hyperlink ref="G38" r:id="rId35"/>
-    <hyperlink ref="G39" r:id="rId36"/>
-    <hyperlink ref="G40" r:id="rId37"/>
-    <hyperlink ref="G41" r:id="rId38"/>
-    <hyperlink ref="G42" r:id="rId39"/>
-    <hyperlink ref="G43" r:id="rId40"/>
-    <hyperlink ref="G44" r:id="rId41"/>
-    <hyperlink ref="G45" r:id="rId42"/>
-    <hyperlink ref="G46" r:id="rId43"/>
-    <hyperlink ref="G47" r:id="rId44"/>
-    <hyperlink ref="G48" r:id="rId45"/>
-    <hyperlink ref="G49" r:id="rId46"/>
-    <hyperlink ref="G50" r:id="rId47"/>
-    <hyperlink ref="G51" r:id="rId48"/>
-    <hyperlink ref="G52" r:id="rId49"/>
-    <hyperlink ref="G53" r:id="rId50"/>
-    <hyperlink ref="G54" r:id="rId51"/>
-    <hyperlink ref="G55" r:id="rId52"/>
-    <hyperlink ref="G56" r:id="rId53"/>
-    <hyperlink ref="G57" r:id="rId54"/>
-    <hyperlink ref="G58" r:id="rId55"/>
-    <hyperlink ref="G59" r:id="rId56"/>
-    <hyperlink ref="G60" r:id="rId57"/>
-    <hyperlink ref="G61" r:id="rId58"/>
-    <hyperlink ref="G62" r:id="rId59"/>
-    <hyperlink ref="G63" r:id="rId60"/>
-    <hyperlink ref="G64" r:id="rId61"/>
-    <hyperlink ref="G65" r:id="rId62"/>
-    <hyperlink ref="G66" r:id="rId63"/>
-    <hyperlink ref="G67" r:id="rId64"/>
-    <hyperlink ref="G68" r:id="rId65"/>
-    <hyperlink ref="G69" r:id="rId66"/>
-    <hyperlink ref="G70" r:id="rId67"/>
-    <hyperlink ref="G71" r:id="rId68"/>
-    <hyperlink ref="G72" r:id="rId69"/>
-    <hyperlink ref="G73" r:id="rId70"/>
-    <hyperlink ref="G74" r:id="rId71"/>
-    <hyperlink ref="G75" r:id="rId72"/>
-    <hyperlink ref="G76" r:id="rId73"/>
-    <hyperlink ref="G77" r:id="rId74"/>
-    <hyperlink ref="G78" r:id="rId75"/>
-    <hyperlink ref="G79" r:id="rId76"/>
-    <hyperlink ref="G80" r:id="rId77"/>
-    <hyperlink ref="G81" r:id="rId78"/>
-    <hyperlink ref="G82" r:id="rId79"/>
-    <hyperlink ref="G83" r:id="rId80"/>
-    <hyperlink ref="G84" r:id="rId81"/>
-    <hyperlink ref="G85" r:id="rId82"/>
-    <hyperlink ref="G86" r:id="rId83"/>
-    <hyperlink ref="G87" r:id="rId84"/>
-    <hyperlink ref="G88" r:id="rId85"/>
-    <hyperlink ref="G89" r:id="rId86"/>
-    <hyperlink ref="G90" r:id="rId87"/>
-    <hyperlink ref="G92" r:id="rId88"/>
-    <hyperlink ref="G93" r:id="rId89"/>
-    <hyperlink ref="G94" r:id="rId90"/>
-    <hyperlink ref="G95" r:id="rId91"/>
-    <hyperlink ref="G96" r:id="rId92"/>
-    <hyperlink ref="G97" r:id="rId93"/>
-    <hyperlink ref="G98" r:id="rId94"/>
-    <hyperlink ref="G99" r:id="rId95"/>
-    <hyperlink ref="G101" r:id="rId96"/>
-    <hyperlink ref="G102" r:id="rId97"/>
-    <hyperlink ref="G103" r:id="rId98"/>
-    <hyperlink ref="G104" r:id="rId99"/>
-    <hyperlink ref="G105" r:id="rId100"/>
-    <hyperlink ref="G106" r:id="rId101"/>
-    <hyperlink ref="G107" r:id="rId102"/>
-    <hyperlink ref="G108" r:id="rId103"/>
-    <hyperlink ref="G109" r:id="rId104"/>
-    <hyperlink ref="G110" r:id="rId105"/>
-    <hyperlink ref="G111" r:id="rId106"/>
-    <hyperlink ref="G112" r:id="rId107"/>
-    <hyperlink ref="G113" r:id="rId108"/>
-    <hyperlink ref="G114" r:id="rId109"/>
-    <hyperlink ref="G115" r:id="rId110"/>
-    <hyperlink ref="G116" r:id="rId111"/>
-    <hyperlink ref="G117" r:id="rId112"/>
-    <hyperlink ref="G118" r:id="rId113"/>
-    <hyperlink ref="G119" r:id="rId114"/>
-    <hyperlink ref="G120" r:id="rId115"/>
-    <hyperlink ref="G121" r:id="rId116"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G25" r:id="rId24"/>
+    <hyperlink ref="G26" r:id="rId25"/>
+    <hyperlink ref="G27" r:id="rId26"/>
+    <hyperlink ref="G28" r:id="rId27"/>
+    <hyperlink ref="G29" r:id="rId28"/>
+    <hyperlink ref="G30" r:id="rId29"/>
+    <hyperlink ref="G31" r:id="rId30"/>
+    <hyperlink ref="G32" r:id="rId31"/>
+    <hyperlink ref="G33" r:id="rId32"/>
+    <hyperlink ref="G34" r:id="rId33"/>
+    <hyperlink ref="G35" r:id="rId34"/>
+    <hyperlink ref="G36" r:id="rId35"/>
+    <hyperlink ref="G37" r:id="rId36"/>
+    <hyperlink ref="G38" r:id="rId37"/>
+    <hyperlink ref="G39" r:id="rId38"/>
+    <hyperlink ref="G40" r:id="rId39"/>
+    <hyperlink ref="G41" r:id="rId40"/>
+    <hyperlink ref="G42" r:id="rId41"/>
+    <hyperlink ref="G43" r:id="rId42"/>
+    <hyperlink ref="G44" r:id="rId43"/>
+    <hyperlink ref="G45" r:id="rId44"/>
+    <hyperlink ref="G46" r:id="rId45"/>
+    <hyperlink ref="G47" r:id="rId46"/>
+    <hyperlink ref="G48" r:id="rId47"/>
+    <hyperlink ref="G49" r:id="rId48"/>
+    <hyperlink ref="G50" r:id="rId49"/>
+    <hyperlink ref="G51" r:id="rId50"/>
+    <hyperlink ref="G52" r:id="rId51"/>
+    <hyperlink ref="G53" r:id="rId52"/>
+    <hyperlink ref="G54" r:id="rId53"/>
+    <hyperlink ref="G55" r:id="rId54"/>
+    <hyperlink ref="G56" r:id="rId55"/>
+    <hyperlink ref="G57" r:id="rId56"/>
+    <hyperlink ref="G58" r:id="rId57"/>
+    <hyperlink ref="G59" r:id="rId58"/>
+    <hyperlink ref="G60" r:id="rId59"/>
+    <hyperlink ref="G61" r:id="rId60"/>
+    <hyperlink ref="G62" r:id="rId61"/>
+    <hyperlink ref="G63" r:id="rId62"/>
+    <hyperlink ref="G64" r:id="rId63"/>
+    <hyperlink ref="G65" r:id="rId64"/>
+    <hyperlink ref="G66" r:id="rId65"/>
+    <hyperlink ref="G67" r:id="rId66"/>
+    <hyperlink ref="G68" r:id="rId67"/>
+    <hyperlink ref="G69" r:id="rId68"/>
+    <hyperlink ref="G70" r:id="rId69"/>
+    <hyperlink ref="G71" r:id="rId70"/>
+    <hyperlink ref="G72" r:id="rId71"/>
+    <hyperlink ref="G73" r:id="rId72"/>
+    <hyperlink ref="G74" r:id="rId73"/>
+    <hyperlink ref="G75" r:id="rId74"/>
+    <hyperlink ref="G76" r:id="rId75"/>
+    <hyperlink ref="G77" r:id="rId76"/>
+    <hyperlink ref="G78" r:id="rId77"/>
+    <hyperlink ref="G79" r:id="rId78"/>
+    <hyperlink ref="G80" r:id="rId79"/>
+    <hyperlink ref="G81" r:id="rId80"/>
+    <hyperlink ref="G82" r:id="rId81"/>
+    <hyperlink ref="G83" r:id="rId82"/>
+    <hyperlink ref="G84" r:id="rId83"/>
+    <hyperlink ref="G85" r:id="rId84"/>
+    <hyperlink ref="G86" r:id="rId85"/>
+    <hyperlink ref="G87" r:id="rId86"/>
+    <hyperlink ref="G88" r:id="rId87"/>
+    <hyperlink ref="G89" r:id="rId88"/>
+    <hyperlink ref="G90" r:id="rId89"/>
+    <hyperlink ref="G91" r:id="rId90"/>
+    <hyperlink ref="G92" r:id="rId91"/>
+    <hyperlink ref="G93" r:id="rId92"/>
+    <hyperlink ref="G94" r:id="rId93"/>
+    <hyperlink ref="G95" r:id="rId94"/>
+    <hyperlink ref="G96" r:id="rId95"/>
+    <hyperlink ref="G97" r:id="rId96"/>
+    <hyperlink ref="G98" r:id="rId97"/>
+    <hyperlink ref="G99" r:id="rId98"/>
+    <hyperlink ref="G100" r:id="rId99"/>
+    <hyperlink ref="G101" r:id="rId100"/>
+    <hyperlink ref="G102" r:id="rId101"/>
+    <hyperlink ref="G103" r:id="rId102"/>
+    <hyperlink ref="G104" r:id="rId103"/>
+    <hyperlink ref="G105" r:id="rId104"/>
+    <hyperlink ref="G106" r:id="rId105"/>
+    <hyperlink ref="G107" r:id="rId106"/>
+    <hyperlink ref="G108" r:id="rId107"/>
+    <hyperlink ref="G109" r:id="rId108"/>
+    <hyperlink ref="G110" r:id="rId109"/>
+    <hyperlink ref="G111" r:id="rId110"/>
+    <hyperlink ref="G112" r:id="rId111"/>
+    <hyperlink ref="G113" r:id="rId112"/>
+    <hyperlink ref="G114" r:id="rId113"/>
+    <hyperlink ref="G115" r:id="rId114"/>
+    <hyperlink ref="G116" r:id="rId115"/>
+    <hyperlink ref="G117" r:id="rId116"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>